<commit_message>
added files for pr and f1f2
</commit_message>
<xml_diff>
--- a/data/larval_pi_curves/PAR_worksheet.xlsx
+++ b/data/larval_pi_curves/PAR_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/larval_symbiont_TPC/data/larval_pi_curves/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390CD506-A1CC-1E47-B947-F336CE5AF745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD794DB-E904-5C4E-AA67-87929FCDCBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17440" xr2:uid="{398F8A14-8E3D-7B41-9975-09624369AC0B}"/>
   </bookViews>
@@ -1448,7 +1448,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1669,8 +1669,13 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
+      <c r="M16" s="3">
+        <v>500</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="0"/>
+        <v>30.15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>